<commit_message>
Implemented inheritance ED and associated tests
Updated the ED formula Excel sheet to allow playing with how it works. Code should allow this form of ED to work in lieu of the existing formula when parent samples are provided, but this hasn't been practically tested yet. Also, I would like to allow both types of results to coexist and to choose which to plot later if both exist.
</commit_message>
<xml_diff>
--- a/tests/ed_formula.xlsx
+++ b/tests/ed_formula.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\psqtl_evaluation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\psQTL\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{473D170F-C592-4F06-AB04-7CE4FCB6117A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD1EFC1B-C831-43F2-ADEC-23E17BB00486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15750" yWindow="1245" windowWidth="21855" windowHeight="15225" xr2:uid="{3C0A386D-72E7-483D-862B-5585D01B21AA}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3C0A386D-72E7-483D-862B-5585D01B21AA}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="segregant_ed" sheetId="1" r:id="rId1"/>
+    <sheet name="inheritance_ed_diploid" sheetId="2" r:id="rId2"/>
+    <sheet name="inheritance_ed_tetraploid" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="35">
   <si>
     <t>A</t>
   </si>
@@ -75,6 +77,72 @@
   </si>
   <si>
     <t>Power 4</t>
+  </si>
+  <si>
+    <t>P1H1</t>
+  </si>
+  <si>
+    <t>P1H2</t>
+  </si>
+  <si>
+    <t>P2H1</t>
+  </si>
+  <si>
+    <t>P2H2</t>
+  </si>
+  <si>
+    <t>0,2</t>
+  </si>
+  <si>
+    <t>1,2</t>
+  </si>
+  <si>
+    <t>0,0</t>
+  </si>
+  <si>
+    <t>0,1</t>
+  </si>
+  <si>
+    <t>Assign '2', then exclude P2H1 allele as assignable. Assign '0' to remaining option.</t>
+  </si>
+  <si>
+    <t>Assign '2', then exclude P2H1 allele as assignable. Assign '1' to remaining option.</t>
+  </si>
+  <si>
+    <t>Partially assign (0.5) to P1H2 and P2H1 for first allele. Partially assign (0.5) likewise for the second allele.</t>
+  </si>
+  <si>
+    <t>Assign '1', then exclude P1H2 as assignable. Assign '0' to remaining option.</t>
+  </si>
+  <si>
+    <t>Column Sum</t>
+  </si>
+  <si>
+    <t>Distance</t>
+  </si>
+  <si>
+    <t>P1H3</t>
+  </si>
+  <si>
+    <t>P1H4</t>
+  </si>
+  <si>
+    <t>P2H3</t>
+  </si>
+  <si>
+    <t>P2H4</t>
+  </si>
+  <si>
+    <t>0,1,2,4</t>
+  </si>
+  <si>
+    <t>0,1,3,5</t>
+  </si>
+  <si>
+    <t>Assign '4', then assign '2'. Partially assign (0.5) for '0' to both parents. Partially assign (0.5) for '1' to both parents.</t>
+  </si>
+  <si>
+    <t>Assign '5', then assign '3'. Partially assign (0.5) for '0' to both parents. Partially assign (0.5) for '1' to both parents.</t>
   </si>
 </sst>
 </file>
@@ -110,8 +178,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -610,4 +681,853 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2FD7944-D890-4E6F-9322-4D21710D0869}">
+  <dimension ref="A1:L10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="H1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8">
+        <f>SUM(B4:B7)/4</f>
+        <v>0.75</v>
+      </c>
+      <c r="C8">
+        <f t="shared" ref="C8:E8" si="0">SUM(C4:C7)/4</f>
+        <v>0.25</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>0.75</v>
+      </c>
+      <c r="H8">
+        <f t="shared" ref="H8" si="1">SUM(H4:H7)/4</f>
+        <v>0.5</v>
+      </c>
+      <c r="I8">
+        <f t="shared" ref="I8" si="2">SUM(I4:I7)/4</f>
+        <v>0.5</v>
+      </c>
+      <c r="J8">
+        <f t="shared" ref="J8" si="3">SUM(J4:J7)/4</f>
+        <v>0.75</v>
+      </c>
+      <c r="K8">
+        <f t="shared" ref="K8" si="4">SUM(K4:K7)/4</f>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9">
+        <f>POWER(B8-H8, 2)</f>
+        <v>6.25E-2</v>
+      </c>
+      <c r="C9">
+        <f t="shared" ref="C9:E9" si="5">POWER(C8-I8, 2)</f>
+        <v>6.25E-2</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="5"/>
+        <v>0.25</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="5"/>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <f>SQRT(SUM(B9:E9)/2)</f>
+        <v>0.55901699437494745</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="H1:K1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25BE4A4D-25E1-4E6D-BA6E-98E36D13BD65}">
+  <dimension ref="A1:T20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="L1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" t="s">
+        <v>30</v>
+      </c>
+      <c r="L2" t="s">
+        <v>13</v>
+      </c>
+      <c r="M2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O2" t="s">
+        <v>28</v>
+      </c>
+      <c r="P2" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>16</v>
+      </c>
+      <c r="R2" t="s">
+        <v>29</v>
+      </c>
+      <c r="S2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>4</v>
+      </c>
+      <c r="I3">
+        <v>5</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>2</v>
+      </c>
+      <c r="O3">
+        <v>3</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>1</v>
+      </c>
+      <c r="R3">
+        <v>4</v>
+      </c>
+      <c r="S3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4">
+        <v>0.5</v>
+      </c>
+      <c r="C4">
+        <v>0.5</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0.5</v>
+      </c>
+      <c r="G4">
+        <v>0.5</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4" t="s">
+        <v>33</v>
+      </c>
+      <c r="K4" t="s">
+        <v>32</v>
+      </c>
+      <c r="L4">
+        <v>0.5</v>
+      </c>
+      <c r="M4">
+        <v>0.5</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>1</v>
+      </c>
+      <c r="P4">
+        <v>0.5</v>
+      </c>
+      <c r="Q4">
+        <v>0.5</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>1</v>
+      </c>
+      <c r="T4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5">
+        <v>0.5</v>
+      </c>
+      <c r="C5">
+        <v>0.5</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0.5</v>
+      </c>
+      <c r="G5">
+        <v>0.5</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5" t="s">
+        <v>33</v>
+      </c>
+      <c r="K5" t="s">
+        <v>32</v>
+      </c>
+      <c r="L5">
+        <v>0.5</v>
+      </c>
+      <c r="M5">
+        <v>0.5</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>1</v>
+      </c>
+      <c r="P5">
+        <v>0.5</v>
+      </c>
+      <c r="Q5">
+        <v>0.5</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>1</v>
+      </c>
+      <c r="T5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6">
+        <v>0.5</v>
+      </c>
+      <c r="C6">
+        <v>0.5</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0.5</v>
+      </c>
+      <c r="G6">
+        <v>0.5</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6" t="s">
+        <v>33</v>
+      </c>
+      <c r="K6" t="s">
+        <v>32</v>
+      </c>
+      <c r="L6">
+        <v>0.5</v>
+      </c>
+      <c r="M6">
+        <v>0.5</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>1</v>
+      </c>
+      <c r="P6">
+        <v>0.5</v>
+      </c>
+      <c r="Q6">
+        <v>0.5</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <v>1</v>
+      </c>
+      <c r="T6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7">
+        <v>0.5</v>
+      </c>
+      <c r="C7">
+        <v>0.5</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0.5</v>
+      </c>
+      <c r="G7">
+        <v>0.5</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7" t="s">
+        <v>33</v>
+      </c>
+      <c r="K7" t="s">
+        <v>32</v>
+      </c>
+      <c r="L7">
+        <v>0.5</v>
+      </c>
+      <c r="M7">
+        <v>0.5</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>1</v>
+      </c>
+      <c r="P7">
+        <v>0.5</v>
+      </c>
+      <c r="Q7">
+        <v>0.5</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>1</v>
+      </c>
+      <c r="T7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8">
+        <v>0.5</v>
+      </c>
+      <c r="C8">
+        <v>0.5</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0.5</v>
+      </c>
+      <c r="G8">
+        <v>0.5</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10">
+        <f>SUM(B4:B8)/5</f>
+        <v>0.5</v>
+      </c>
+      <c r="C10">
+        <f t="shared" ref="C10:I10" si="0">SUM(C4:C8)/5</f>
+        <v>0.5</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <f>SUM(L4:L7)/4</f>
+        <v>0.5</v>
+      </c>
+      <c r="M10">
+        <f t="shared" ref="M10" si="1">SUM(M4:M7)/4</f>
+        <v>0.5</v>
+      </c>
+      <c r="N10">
+        <f>SUM(N4:N7)/4</f>
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <f>SUM(O4:O7)/4</f>
+        <v>1</v>
+      </c>
+      <c r="P10">
+        <f t="shared" ref="P10:S10" si="2">SUM(P4:P7)/4</f>
+        <v>0.5</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="R10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11">
+        <f>POWER(B10-L10, 2)</f>
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <f t="shared" ref="C11:I11" si="3">POWER(C10-M10, 2)</f>
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <f>SQRT(SUM(B11:I11)/2)</f>
+        <v>1.4142135623730951</v>
+      </c>
+    </row>
+    <row r="20" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="L1:S1"/>
+    <mergeCell ref="L20:O20"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>